<commit_message>
first edition of multi-factors-model
</commit_message>
<xml_diff>
--- a/参数整理.xlsx
+++ b/参数整理.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20760" windowHeight="11190" tabRatio="685" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20760" windowHeight="11190" tabRatio="685"/>
   </bookViews>
   <sheets>
     <sheet name="指标解释" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
   <externalReferences>
     <externalReference r:id="rId6"/>
   </externalReferences>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -641,7 +641,7 @@
     <numFmt numFmtId="176" formatCode="yyyy&quot;年&quot;m&quot;月&quot;;@"/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -851,7 +851,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1553,13 +1552,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="479104000"/>
-        <c:axId val="182702848"/>
+        <c:axId val="512873200"/>
+        <c:axId val="512873760"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="479104000"/>
+        <c:axId val="512873200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1602,14 +1600,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="182702848"/>
+        <c:crossAx val="512873760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="182702848"/>
+        <c:axId val="512873760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1660,7 +1658,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479104000"/>
+        <c:crossAx val="512873200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1880,11 +1878,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="205677312"/>
-        <c:axId val="205678848"/>
+        <c:axId val="512876000"/>
+        <c:axId val="512876560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="205677312"/>
+        <c:axId val="512876000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1927,7 +1925,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="205678848"/>
+        <c:crossAx val="512876560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1935,7 +1933,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="205678848"/>
+        <c:axId val="512876560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1986,7 +1984,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="205677312"/>
+        <c:crossAx val="512876000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3220,7 +3218,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3262,7 +3260,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3297,7 +3295,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3508,11 +3506,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.75" style="2" bestFit="1" customWidth="1"/>
@@ -3520,7 +3518,7 @@
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3531,7 +3529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -3539,7 +3537,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -3547,7 +3545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -3555,7 +3553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3563,7 +3561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
@@ -3571,7 +3569,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
@@ -3579,7 +3577,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>15</v>
@@ -3588,7 +3586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -3599,7 +3597,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B10" s="2" t="s">
         <v>94</v>
       </c>
@@ -3607,7 +3605,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
         <v>95</v>
       </c>
@@ -3615,7 +3613,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
         <v>96</v>
@@ -3624,7 +3622,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -3635,7 +3633,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B14" s="2" t="s">
         <v>98</v>
       </c>
@@ -3643,7 +3641,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B15" s="2" t="s">
         <v>99</v>
       </c>
@@ -3651,7 +3649,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B16" s="2" t="s">
         <v>100</v>
       </c>
@@ -3659,7 +3657,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B17" s="2" t="s">
         <v>101</v>
       </c>
@@ -3667,7 +3665,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B18" s="2" t="s">
         <v>102</v>
       </c>
@@ -3675,7 +3673,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B19" s="2" t="s">
         <v>103</v>
       </c>
@@ -3683,7 +3681,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B20" s="2" t="s">
         <v>104</v>
       </c>
@@ -3691,7 +3689,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
         <v>105</v>
       </c>
@@ -3699,7 +3697,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B22" s="2" t="s">
         <v>106</v>
       </c>
@@ -3707,7 +3705,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B23" s="2" t="s">
         <v>107</v>
       </c>
@@ -3715,7 +3713,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
         <v>108</v>
@@ -3724,7 +3722,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>74</v>
       </c>
@@ -3735,7 +3733,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B26" s="2" t="s">
         <v>34</v>
       </c>
@@ -3743,7 +3741,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B27" s="2" t="s">
         <v>35</v>
       </c>
@@ -3751,7 +3749,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
         <v>36</v>
@@ -3760,7 +3758,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>79</v>
       </c>
@@ -3771,7 +3769,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>121</v>
       </c>
@@ -3782,7 +3780,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B31" s="2" t="s">
         <v>38</v>
       </c>
@@ -3790,7 +3788,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B32" s="2" t="s">
         <v>39</v>
       </c>
@@ -3798,7 +3796,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B33" s="2" t="s">
         <v>40</v>
       </c>
@@ -3806,7 +3804,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B34" s="2" t="s">
         <v>41</v>
       </c>
@@ -3814,7 +3812,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="24">
+    <row r="35" spans="2:3" ht="24" x14ac:dyDescent="0.15">
       <c r="B35" s="2" t="s">
         <v>42</v>
       </c>
@@ -3822,7 +3820,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="24">
+    <row r="36" spans="2:3" ht="24" x14ac:dyDescent="0.15">
       <c r="B36" s="2" t="s">
         <v>43</v>
       </c>
@@ -3830,7 +3828,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="2:3" ht="24">
+    <row r="37" spans="2:3" ht="24" x14ac:dyDescent="0.15">
       <c r="B37" s="2" t="s">
         <v>44</v>
       </c>
@@ -3838,7 +3836,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="24">
+    <row r="38" spans="2:3" ht="24" x14ac:dyDescent="0.15">
       <c r="B38" s="2" t="s">
         <v>45</v>
       </c>
@@ -3846,7 +3844,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="2:3" ht="36">
+    <row r="39" spans="2:3" ht="36" x14ac:dyDescent="0.15">
       <c r="B39" s="2" t="s">
         <v>46</v>
       </c>
@@ -3854,7 +3852,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="2:3" ht="36">
+    <row r="40" spans="2:3" ht="36" x14ac:dyDescent="0.15">
       <c r="B40" s="2" t="s">
         <v>47</v>
       </c>
@@ -3862,7 +3860,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="2:3" ht="36">
+    <row r="41" spans="2:3" ht="36" x14ac:dyDescent="0.15">
       <c r="B41" s="2" t="s">
         <v>48</v>
       </c>
@@ -3870,7 +3868,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="2:3" ht="36">
+    <row r="42" spans="2:3" ht="36" x14ac:dyDescent="0.15">
       <c r="B42" s="2" t="s">
         <v>49</v>
       </c>
@@ -3878,7 +3876,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="2:3" ht="24">
+    <row r="43" spans="2:3" ht="24" x14ac:dyDescent="0.15">
       <c r="B43" s="2" t="s">
         <v>109</v>
       </c>
@@ -3886,7 +3884,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" spans="2:3" ht="24">
+    <row r="44" spans="2:3" ht="24" x14ac:dyDescent="0.15">
       <c r="B44" s="2" t="s">
         <v>110</v>
       </c>
@@ -3894,7 +3892,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="2:3" ht="24">
+    <row r="45" spans="2:3" ht="24" x14ac:dyDescent="0.15">
       <c r="B45" s="2" t="s">
         <v>111</v>
       </c>
@@ -3902,7 +3900,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="2:3" ht="24">
+    <row r="46" spans="2:3" ht="24" x14ac:dyDescent="0.15">
       <c r="B46" s="2" t="s">
         <v>112</v>
       </c>
@@ -3910,7 +3908,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="2:3">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B47" s="2" t="s">
         <v>50</v>
       </c>
@@ -3918,7 +3916,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="2:3">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B48" s="2" t="s">
         <v>51</v>
       </c>
@@ -3926,7 +3924,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B49" s="2" t="s">
         <v>52</v>
       </c>
@@ -3934,7 +3932,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50" s="4"/>
       <c r="B50" s="4" t="s">
         <v>53</v>
@@ -3943,7 +3941,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" s="6" t="s">
         <v>122</v>
       </c>
@@ -3954,7 +3952,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" s="4" t="s">
         <v>124</v>
       </c>
@@ -3965,7 +3963,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
         <v>126</v>
       </c>
@@ -3976,7 +3974,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B54" s="2" t="s">
         <v>56</v>
       </c>
@@ -3984,7 +3982,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B55" s="2" t="s">
         <v>57</v>
       </c>
@@ -3992,7 +3990,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B56" s="2" t="s">
         <v>58</v>
       </c>
@@ -4000,7 +3998,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="24">
+    <row r="57" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="B57" s="2" t="s">
         <v>59</v>
       </c>
@@ -4008,7 +4006,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="24">
+    <row r="58" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="B58" s="2" t="s">
         <v>60</v>
       </c>
@@ -4016,7 +4014,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="24">
+    <row r="59" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="B59" s="2" t="s">
         <v>61</v>
       </c>
@@ -4024,7 +4022,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="24">
+    <row r="60" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A60" s="4"/>
       <c r="B60" s="4" t="s">
         <v>62</v>
@@ -4033,7 +4031,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
         <v>135</v>
       </c>
@@ -4044,7 +4042,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B62" s="2" t="s">
         <v>64</v>
       </c>
@@ -4052,7 +4050,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="4"/>
       <c r="B63" s="4" t="s">
         <v>65</v>
@@ -4061,7 +4059,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="6" t="s">
         <v>139</v>
       </c>
@@ -4072,7 +4070,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="2" t="s">
         <v>141</v>
       </c>
@@ -4083,7 +4081,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B66" s="2" t="s">
         <v>67</v>
       </c>
@@ -4091,7 +4089,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B67" s="2" t="s">
         <v>68</v>
       </c>
@@ -4099,7 +4097,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B68" s="2" t="s">
         <v>69</v>
       </c>
@@ -4107,7 +4105,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B69" s="2" t="s">
         <v>70</v>
       </c>
@@ -4115,7 +4113,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A70" s="4"/>
       <c r="B70" s="4" t="s">
         <v>71</v>
@@ -4138,7 +4136,7 @@
       <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="32.75" style="1" bestFit="1" customWidth="1"/>
@@ -4149,7 +4147,7 @@
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="str">
         <f>IF(指标解释!A1&gt;0,指标解释!A1,"")</f>
         <v>估值因子</v>
@@ -4167,7 +4165,7 @@
         <v>净利润(TTM)/总市值</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="str">
         <f>IF(指标解释!A2&gt;0,指标解释!A2,"")</f>
         <v/>
@@ -4185,7 +4183,7 @@
         <v>扣非后净利润(TTM)/总市值</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="str">
         <f>IF(指标解释!A3&gt;0,指标解释!A3,"")</f>
         <v/>
@@ -4203,7 +4201,7 @@
         <v>净资产/总市值</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="str">
         <f>IF(指标解释!A4&gt;0,指标解释!A4,"")</f>
         <v/>
@@ -4221,7 +4219,7 @@
         <v>营业收入(TTM)/总市值</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="str">
         <f>IF(指标解释!A5&gt;0,指标解释!A5,"")</f>
         <v/>
@@ -4239,7 +4237,7 @@
         <v>净现金流(TTM)/总市值</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="str">
         <f>IF(指标解释!A6&gt;0,指标解释!A6,"")</f>
         <v/>
@@ -4257,7 +4255,7 @@
         <v>经营性现金流(TTM)/总市值</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="str">
         <f>IF(指标解释!A7&gt;0,指标解释!A7,"")</f>
         <v/>
@@ -4275,7 +4273,7 @@
         <v>近12个月现金红利(按除息日计)/总市值</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="str">
         <f>IF(指标解释!A8&gt;0,指标解释!A8,"")</f>
         <v/>
@@ -4293,7 +4291,7 @@
         <v>净利润(TTM)同比增长率/PE(TTM)</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="str">
         <f>IF(指标解释!A9&gt;0,指标解释!A9,"")</f>
         <v>成长因子</v>
@@ -4311,7 +4309,7 @@
         <v>营业收入(最新财报，YTD)同比增长率</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="str">
         <f>IF(指标解释!A10&gt;0,指标解释!A10,"")</f>
         <v/>
@@ -4329,7 +4327,7 @@
         <v>净利润(最新财报，YTD)同比增长率</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="str">
         <f>IF(指标解释!A11&gt;0,指标解释!A11,"")</f>
         <v/>
@@ -4347,7 +4345,7 @@
         <v>经营性现金流(最新财报，YTD)同比增长率</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="str">
         <f>IF(指标解释!A12&gt;0,指标解释!A12,"")</f>
         <v/>
@@ -4365,7 +4363,7 @@
         <v>ROE(最新财报，YTD)同比增长率</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="str">
         <f>IF(指标解释!A13&gt;0,指标解释!A13,"")</f>
         <v>财务质量</v>
@@ -4383,7 +4381,7 @@
         <v>ROE(最新财报，YTD)</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="str">
         <f>IF(指标解释!A14&gt;0,指标解释!A14,"")</f>
         <v/>
@@ -4401,7 +4399,7 @@
         <v>ROE(最新财报，TTM)</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="str">
         <f>IF(指标解释!A15&gt;0,指标解释!A15,"")</f>
         <v/>
@@ -4419,7 +4417,7 @@
         <v>ROA(最新财报，YTD)</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="str">
         <f>IF(指标解释!A16&gt;0,指标解释!A16,"")</f>
         <v/>
@@ -4437,7 +4435,7 @@
         <v>ROE(最新财报，TTM)</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="str">
         <f>IF(指标解释!A17&gt;0,指标解释!A17,"")</f>
         <v/>
@@ -4455,7 +4453,7 @@
         <v>毛利率(最新财报，YTD)</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="str">
         <f>IF(指标解释!A18&gt;0,指标解释!A18,"")</f>
         <v/>
@@ -4473,7 +4471,7 @@
         <v>毛利率(最新财报，TTM)</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="str">
         <f>IF(指标解释!A19&gt;0,指标解释!A19,"")</f>
         <v/>
@@ -4491,7 +4489,7 @@
         <v>扣非后净利润率(最新财报，YTD)</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="str">
         <f>IF(指标解释!A20&gt;0,指标解释!A20,"")</f>
         <v/>
@@ -4509,7 +4507,7 @@
         <v>扣非后净利润率(最新财报，TTM)</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="str">
         <f>IF(指标解释!A21&gt;0,指标解释!A21,"")</f>
         <v/>
@@ -4527,7 +4525,7 @@
         <v>资产周转率(最新财报，YTD)</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="str">
         <f>IF(指标解释!A22&gt;0,指标解释!A22,"")</f>
         <v/>
@@ -4545,7 +4543,7 @@
         <v>资产周转率(最新财报，TTM)</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="str">
         <f>IF(指标解释!A23&gt;0,指标解释!A23,"")</f>
         <v/>
@@ -4563,7 +4561,7 @@
         <v>经营性现金流/净利润(最新财报，YTD)</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="str">
         <f>IF(指标解释!A24&gt;0,指标解释!A24,"")</f>
         <v/>
@@ -4581,7 +4579,7 @@
         <v>经营性现金流/净利润(最新财报，TTM)</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="str">
         <f>IF(指标解释!A25&gt;0,指标解释!A25,"")</f>
         <v>杠杆因子</v>
@@ -4599,7 +4597,7 @@
         <v>总资产/净资产</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="str">
         <f>IF(指标解释!A26&gt;0,指标解释!A26,"")</f>
         <v/>
@@ -4617,7 +4615,7 @@
         <v>非流动资产/净资产</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="str">
         <f>IF(指标解释!A27&gt;0,指标解释!A27,"")</f>
         <v/>
@@ -4635,7 +4633,7 @@
         <v>现金比率</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="str">
         <f>IF(指标解释!A28&gt;0,指标解释!A28,"")</f>
         <v/>
@@ -4653,7 +4651,7 @@
         <v>流动比率</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="str">
         <f>IF(指标解释!A29&gt;0,指标解释!A29,"")</f>
         <v>市值</v>
@@ -4671,7 +4669,7 @@
         <v>总市值取对数</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="str">
         <f>IF(指标解释!A30&gt;0,指标解释!A30,"")</f>
         <v>动量反转</v>
@@ -4689,7 +4687,7 @@
         <v>个股60个月收益与上证综指回归的截距项</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="str">
         <f>IF(指标解释!A31&gt;0,指标解释!A31,"")</f>
         <v/>
@@ -4707,7 +4705,7 @@
         <v>个股最近1个月收益率</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="str">
         <f>IF(指标解释!A32&gt;0,指标解释!A32,"")</f>
         <v/>
@@ -4725,7 +4723,7 @@
         <v>个股最近3个月收益率</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="str">
         <f>IF(指标解释!A33&gt;0,指标解释!A33,"")</f>
         <v/>
@@ -4743,7 +4741,7 @@
         <v>个股最近6个月收益率</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="str">
         <f>IF(指标解释!A34&gt;0,指标解释!A34,"")</f>
         <v/>
@@ -4761,7 +4759,7 @@
         <v>个股最近12个月收益率</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="str">
         <f>IF(指标解释!A35&gt;0,指标解释!A35,"")</f>
         <v/>
@@ -4779,7 +4777,7 @@
         <v>个股近1个月内“每日换手率*每日收益率”的算术平均值</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="str">
         <f>IF(指标解释!A36&gt;0,指标解释!A36,"")</f>
         <v/>
@@ -4797,7 +4795,7 @@
         <v>个股近3个月内“每日换手率*每日收益率”的算术平均值</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="str">
         <f>IF(指标解释!A37&gt;0,指标解释!A37,"")</f>
         <v/>
@@ -4815,7 +4813,7 @@
         <v>个股近6个月内“每日换手率*每日收益率”的算术平均值</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="str">
         <f>IF(指标解释!A38&gt;0,指标解释!A38,"")</f>
         <v/>
@@ -4833,7 +4831,7 @@
         <v>个股近12个月内“每日换手率*每日收益率”的算术平均值</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="str">
         <f>IF(指标解释!A39&gt;0,指标解释!A39,"")</f>
         <v/>
@@ -4851,7 +4849,7 @@
         <v>个股最近1个月“每日换手率*exp(-x_1/N/4)*每日收益率）”的算术平均值，x_1为该日距离截面日的交易日个数</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="str">
         <f>IF(指标解释!A40&gt;0,指标解释!A40,"")</f>
         <v/>
@@ -4869,7 +4867,7 @@
         <v>个股最近3个月“每日换手率*exp(-x_1/N/4)*每日收益率）”的算术平均值，x_1为该日距离截面日的交易日个数</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="str">
         <f>IF(指标解释!A41&gt;0,指标解释!A41,"")</f>
         <v/>
@@ -4887,7 +4885,7 @@
         <v>个股最近6个月“每日换手率*exp(-x_1/N/4)*每日收益率）”的算术平均值，x_1为该日距离截面日的交易日个数</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="str">
         <f>IF(指标解释!A42&gt;0,指标解释!A42,"")</f>
         <v/>
@@ -4905,7 +4903,7 @@
         <v>个股最近12个月“每日换手率*exp(-x_1/N/4)*每日收益率）”的算术平均值，x_1为该日距离截面日的交易日个数</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="str">
         <f>IF(指标解释!A43&gt;0,指标解释!A43,"")</f>
         <v/>
@@ -4923,7 +4921,7 @@
         <v>特质波动率：个股最近1个月内用日频收益率对Fama French三因子回归的残差的标准差</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="str">
         <f>IF(指标解释!A44&gt;0,指标解释!A44,"")</f>
         <v/>
@@ -4941,7 +4939,7 @@
         <v>特质波动率：个股最近3个月内用日频收益率对Fama French三因子回归的残差的标准差</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="str">
         <f>IF(指标解释!A45&gt;0,指标解释!A45,"")</f>
         <v/>
@@ -4959,7 +4957,7 @@
         <v>特质波动率：个股最近6个月内用日频收益率对Fama French三因子回归的残差的标准差</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="str">
         <f>IF(指标解释!A46&gt;0,指标解释!A46,"")</f>
         <v/>
@@ -4977,7 +4975,7 @@
         <v>特质波动率：个股最近12个月内用日频收益率对Fama French三因子回归的残差的标准差</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="str">
         <f>IF(指标解释!A47&gt;0,指标解释!A47,"")</f>
         <v/>
@@ -4995,7 +4993,7 @@
         <v>个股最近1个月的日收益标准差</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="str">
         <f>IF(指标解释!A48&gt;0,指标解释!A48,"")</f>
         <v/>
@@ -5013,7 +5011,7 @@
         <v>个股最近3个月的日收益标准差</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="str">
         <f>IF(指标解释!A49&gt;0,指标解释!A49,"")</f>
         <v/>
@@ -5031,7 +5029,7 @@
         <v>个股最近6个月的日收益标准差</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="str">
         <f>IF(指标解释!A50&gt;0,指标解释!A50,"")</f>
         <v/>
@@ -5049,7 +5047,7 @@
         <v>个股最近12个月的日收益标准差</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="str">
         <f>IF(指标解释!A51&gt;0,指标解释!A51,"")</f>
         <v>股价</v>
@@ -5067,7 +5065,7 @@
         <v>股价取对数</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="str">
         <f>IF(指标解释!A52&gt;0,指标解释!A52,"")</f>
         <v>beta</v>
@@ -5085,7 +5083,7 @@
         <v>个股前60个月的收益与上证综指回归的beta</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="str">
         <f>IF(指标解释!A53&gt;0,指标解释!A53,"")</f>
         <v>换手率</v>
@@ -5103,7 +5101,7 @@
         <v>最近1个月日均换手率（剔除停牌、涨跌停）</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="str">
         <f>IF(指标解释!A54&gt;0,指标解释!A54,"")</f>
         <v/>
@@ -5121,7 +5119,7 @@
         <v>最近3个月日均换手率（剔除停牌、涨跌停）</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="str">
         <f>IF(指标解释!A55&gt;0,指标解释!A55,"")</f>
         <v/>
@@ -5139,7 +5137,7 @@
         <v>最近6个月日均换手率（剔除停牌、涨跌停）</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="str">
         <f>IF(指标解释!A56&gt;0,指标解释!A56,"")</f>
         <v/>
@@ -5157,7 +5155,7 @@
         <v>最近12个月日均换手率（剔除停牌、涨跌停）</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="str">
         <f>IF(指标解释!A57&gt;0,指标解释!A57,"")</f>
         <v/>
@@ -5175,7 +5173,7 @@
         <v>个股最近1个月日均换手率除以最近2年日均换手率再减1（剔除停牌、涨跌停）</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="str">
         <f>IF(指标解释!A58&gt;0,指标解释!A58,"")</f>
         <v/>
@@ -5193,7 +5191,7 @@
         <v>个股最近3个月日均换手率除以最近2年日均换手率再减1（剔除停牌、涨跌停）</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="str">
         <f>IF(指标解释!A59&gt;0,指标解释!A59,"")</f>
         <v/>
@@ -5211,7 +5209,7 @@
         <v>个股最近6个月日均换手率除以最近2年日均换手率再减1（剔除停牌、涨跌停）</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="str">
         <f>IF(指标解释!A60&gt;0,指标解释!A60,"")</f>
         <v/>
@@ -5229,7 +5227,7 @@
         <v>个股最近12个月日均换手率除以最近2年日均换手率再减1（剔除停牌、涨跌停）</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="str">
         <f>IF(指标解释!A61&gt;0,指标解释!A61,"")</f>
         <v>情绪</v>
@@ -5247,7 +5245,7 @@
         <v>wind评级的平均值</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="str">
         <f>IF(指标解释!A62&gt;0,指标解释!A62,"")</f>
         <v/>
@@ -5265,7 +5263,7 @@
         <v>wind评级：（上调家数-下调家数）/总家数</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="str">
         <f>IF(指标解释!A63&gt;0,指标解释!A63,"")</f>
         <v/>
@@ -5283,7 +5281,7 @@
         <v>wind一直目标价/现价-1</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="str">
         <f>IF(指标解释!A64&gt;0,指标解释!A64,"")</f>
         <v>股东</v>
@@ -5301,7 +5299,7 @@
         <v>户均持股比例同比增长率</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="str">
         <f>IF(指标解释!A65&gt;0,指标解释!A65,"")</f>
         <v>技术指标</v>
@@ -5319,7 +5317,7 @@
         <v>30日MACD</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="str">
         <f>IF(指标解释!A66&gt;0,指标解释!A66,"")</f>
         <v/>
@@ -5337,7 +5335,7 @@
         <v>15日DEA</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="str">
         <f>IF(指标解释!A67&gt;0,指标解释!A67,"")</f>
         <v/>
@@ -5355,7 +5353,7 @@
         <v>10日DIF</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="str">
         <f>IF(指标解释!A68&gt;0,指标解释!A68,"")</f>
         <v/>
@@ -5373,7 +5371,7 @@
         <v>20日RSI</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="str">
         <f>IF(指标解释!A69&gt;0,指标解释!A69,"")</f>
         <v/>
@@ -5391,7 +5389,7 @@
         <v>20日PSY</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="str">
         <f>IF(指标解释!A70&gt;0,指标解释!A70,"")</f>
         <v/>
@@ -5409,7 +5407,7 @@
         <v>20日BIAS</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B72" s="10" t="s">
         <v>148</v>
       </c>
@@ -5432,7 +5430,7 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.375" style="13" customWidth="1"/>
@@ -5440,14 +5438,14 @@
     <col min="4" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="23" t="s">
         <v>156</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="18"/>
       <c r="B2" s="19" t="s">
         <v>150</v>
@@ -5456,7 +5454,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
         <v>149</v>
       </c>
@@ -5467,12 +5465,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="17"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="15" t="s">
         <v>152</v>
       </c>
@@ -5484,7 +5482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="15" t="s">
         <v>155</v>
       </c>
@@ -5496,12 +5494,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="17"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
         <v>153</v>
       </c>
@@ -5513,7 +5511,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="15" t="s">
         <v>154</v>
       </c>
@@ -5525,27 +5523,27 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C10" s="14">
         <v>242</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C11" s="14">
         <v>241</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C12" s="14">
         <v>240</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C13" s="14">
         <v>239</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C14" s="14">
         <v>238</v>
       </c>
@@ -5567,19 +5565,19 @@
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.25" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.75" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13.5">
+    <row r="2" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A2" s="22">
         <v>40179</v>
       </c>
@@ -5587,7 +5585,7 @@
         <v>1.070792929</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13.5">
+    <row r="3" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A3" s="22">
         <v>40210</v>
       </c>
@@ -5595,7 +5593,7 @@
         <v>1.0959022950458499</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13.5">
+    <row r="4" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A4" s="22">
         <v>40238</v>
       </c>
@@ -5603,7 +5601,7 @@
         <v>1.1696923215345201</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13.5">
+    <row r="5" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A5" s="22">
         <v>40269</v>
       </c>
@@ -5611,7 +5609,7 @@
         <v>1.15983636525014</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13.5">
+    <row r="6" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A6" s="22">
         <v>40299</v>
       </c>
@@ -5619,7 +5617,7 @@
         <v>1.17265028264704</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13.5">
+    <row r="7" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A7" s="22">
         <v>40330</v>
       </c>
@@ -5627,7 +5625,7 @@
         <v>1.23814318790747</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="13.5">
+    <row r="8" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A8" s="22">
         <v>40360</v>
       </c>
@@ -5635,7 +5633,7 @@
         <v>1.2931098390878699</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13.5">
+    <row r="9" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A9" s="22">
         <v>40391</v>
       </c>
@@ -5643,7 +5641,7 @@
         <v>1.3533290591172999</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="13.5">
+    <row r="10" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A10" s="22">
         <v>40422</v>
       </c>
@@ -5651,7 +5649,7 @@
         <v>1.3611158573909401</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="13.5">
+    <row r="11" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A11" s="22">
         <v>40452</v>
       </c>
@@ -5659,7 +5657,7 @@
         <v>1.3354665981728999</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="13.5">
+    <row r="12" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A12" s="22">
         <v>40483</v>
       </c>
@@ -5667,7 +5665,7 @@
         <v>1.2761613685545099</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="13.5">
+    <row r="13" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A13" s="22">
         <v>40513</v>
       </c>
@@ -5675,7 +5673,7 @@
         <v>1.3769558093695899</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="13.5">
+    <row r="14" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A14" s="22">
         <v>40544</v>
       </c>
@@ -5683,7 +5681,7 @@
         <v>1.413875883142</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="13.5">
+    <row r="15" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A15" s="22">
         <v>40575</v>
       </c>
@@ -5691,7 +5689,7 @@
         <v>1.47395999508827</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="13.5">
+    <row r="16" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A16" s="22">
         <v>40603</v>
       </c>
@@ -5699,7 +5697,7 @@
         <v>1.4804459644318599</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="13.5">
+    <row r="17" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A17" s="22">
         <v>40634</v>
       </c>
@@ -5707,7 +5705,7 @@
         <v>1.4958935697751701</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="13.5">
+    <row r="18" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A18" s="22">
         <v>40664</v>
       </c>
@@ -5715,7 +5713,7 @@
         <v>1.54208521645588</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="13.5">
+    <row r="19" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A19" s="22">
         <v>40695</v>
       </c>
@@ -5723,7 +5721,7 @@
         <v>1.5639351159550401</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="13.5">
+    <row r="20" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A20" s="22">
         <v>40725</v>
       </c>
@@ -5731,7 +5729,7 @@
         <v>1.5591266473032599</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="13.5">
+    <row r="21" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A21" s="22">
         <v>40756</v>
       </c>
@@ -5739,7 +5737,7 @@
         <v>1.53847986122517</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="13.5">
+    <row r="22" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A22" s="22">
         <v>40787</v>
       </c>
@@ -5747,7 +5745,7 @@
         <v>1.54603928663993</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="13.5">
+    <row r="23" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A23" s="22">
         <v>40817</v>
       </c>
@@ -5755,7 +5753,7 @@
         <v>1.5380763169856999</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="13.5">
+    <row r="24" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A24" s="22">
         <v>40848</v>
       </c>
@@ -5763,7 +5761,7 @@
         <v>1.4272120221495801</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="13.5">
+    <row r="25" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A25" s="22">
         <v>40878</v>
       </c>
@@ -5771,7 +5769,7 @@
         <v>1.4283196931031099</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="13.5">
+    <row r="26" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A26" s="22">
         <v>40909</v>
       </c>
@@ -5779,7 +5777,7 @@
         <v>1.5548665468837299</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="13.5">
+    <row r="27" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A27" s="22">
         <v>40940</v>
       </c>
@@ -5787,7 +5785,7 @@
         <v>1.56903088356854</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="13.5">
+    <row r="28" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A28" s="22">
         <v>40969</v>
       </c>
@@ -5795,7 +5793,7 @@
         <v>1.5812545033946499</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="13.5">
+    <row r="29" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A29" s="22">
         <v>41000</v>
       </c>
@@ -5803,7 +5801,7 @@
         <v>1.66770031140382</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="13.5">
+    <row r="30" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A30" s="22">
         <v>41030</v>
       </c>
@@ -5811,7 +5809,7 @@
         <v>1.7290420128072399</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="13.5">
+    <row r="31" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A31" s="22">
         <v>41061</v>
       </c>
@@ -5819,7 +5817,7 @@
         <v>1.7792269730972099</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="13.5">
+    <row r="32" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A32" s="22">
         <v>41091</v>
       </c>
@@ -5827,7 +5825,7 @@
         <v>2.0050678290386501</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="13.5">
+    <row r="33" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A33" s="22">
         <v>41122</v>
       </c>
@@ -5835,7 +5833,7 @@
         <v>1.9647866479496301</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="13.5">
+    <row r="34" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A34" s="22">
         <v>41153</v>
       </c>
@@ -5843,7 +5841,7 @@
         <v>2.06424539492245</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="13.5">
+    <row r="35" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A35" s="22">
         <v>41183</v>
       </c>
@@ -5851,7 +5849,7 @@
         <v>1.94409462105205</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="13.5">
+    <row r="36" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A36" s="22">
         <v>41214</v>
       </c>
@@ -5859,7 +5857,7 @@
         <v>2.0286465427596201</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="13.5">
+    <row r="37" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A37" s="22">
         <v>41244</v>
       </c>
@@ -5867,7 +5865,7 @@
         <v>1.99712192119105</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="13.5">
+    <row r="38" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A38" s="22">
         <v>41275</v>
       </c>
@@ -5875,7 +5873,7 @@
         <v>2.1111068340259198</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="13.5">
+    <row r="39" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A39" s="22">
         <v>41306</v>
       </c>
@@ -5883,7 +5881,7 @@
         <v>2.1012534962109299</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="13.5">
+    <row r="40" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A40" s="22">
         <v>41334</v>
       </c>
@@ -5891,7 +5889,7 @@
         <v>2.0470361970504301</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="13.5">
+    <row r="41" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A41" s="22">
         <v>41365</v>
       </c>
@@ -5899,7 +5897,7 @@
         <v>2.2843028198860802</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="13.5">
+    <row r="42" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A42" s="22">
         <v>41395</v>
       </c>
@@ -5907,7 +5905,7 @@
         <v>2.37957439064335</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="13.5">
+    <row r="43" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A43" s="22">
         <v>41426</v>
       </c>
@@ -5915,7 +5913,7 @@
         <v>2.5634399395531799</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="13.5">
+    <row r="44" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A44" s="22">
         <v>41456</v>
       </c>
@@ -5923,7 +5921,7 @@
         <v>2.6716915370444099</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="13.5">
+    <row r="45" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A45" s="22">
         <v>41487</v>
       </c>
@@ -5931,7 +5929,7 @@
         <v>2.7929625440847801</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="13.5">
+    <row r="46" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A46" s="22">
         <v>41518</v>
       </c>
@@ -5939,7 +5937,7 @@
         <v>2.7394335624002699</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="13.5">
+    <row r="47" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A47" s="22">
         <v>41548</v>
       </c>
@@ -5947,7 +5945,7 @@
         <v>2.8090622136989301</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="13.5">
+    <row r="48" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A48" s="22">
         <v>41579</v>
       </c>
@@ -5955,7 +5953,7 @@
         <v>2.9014414943448399</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="13.5">
+    <row r="49" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A49" s="22">
         <v>41609</v>
       </c>
@@ -5963,7 +5961,7 @@
         <v>3.06722998899513</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="13.5">
+    <row r="50" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A50" s="22">
         <v>41640</v>
       </c>
@@ -5971,7 +5969,7 @@
         <v>3.3339785462555702</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="13.5">
+    <row r="51" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A51" s="22">
         <v>41671</v>
       </c>
@@ -5979,7 +5977,7 @@
         <v>3.4224350315889001</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="13.5">
+    <row r="52" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A52" s="22">
         <v>41699</v>
       </c>
@@ -5987,7 +5985,7 @@
         <v>3.3205533160692302</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="13.5">
+    <row r="53" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A53" s="22">
         <v>41730</v>
       </c>
@@ -5995,7 +5993,7 @@
         <v>3.3901364306007302</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="13.5">
+    <row r="54" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A54" s="22">
         <v>41760</v>
       </c>
@@ -6003,7 +6001,7 @@
         <v>3.5726161855056602</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="13.5">
+    <row r="55" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A55" s="22">
         <v>41791</v>
       </c>
@@ -6011,7 +6009,7 @@
         <v>3.59324218202832</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="13.5">
+    <row r="56" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A56" s="22">
         <v>41821</v>
       </c>
@@ -6019,7 +6017,7 @@
         <v>3.8076496207168198</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="13.5">
+    <row r="57" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A57" s="22">
         <v>41852</v>
       </c>
@@ -6027,7 +6025,7 @@
         <v>4.2489377408495903</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="13.5">
+    <row r="58" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A58" s="22">
         <v>41883</v>
       </c>
@@ -6035,7 +6033,7 @@
         <v>4.7087518495227796</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="13.5">
+    <row r="59" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A59" s="22">
         <v>41913</v>
       </c>
@@ -6043,7 +6041,7 @@
         <v>4.5531415388015297</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="13.5">
+    <row r="60" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A60" s="22">
         <v>41944</v>
       </c>
@@ -6051,7 +6049,7 @@
         <v>3.6585351715267098</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="13.5">
+    <row r="61" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A61" s="22">
         <v>41974</v>
       </c>
@@ -6059,7 +6057,7 @@
         <v>4.04693115557762</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="13.5">
+    <row r="62" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A62" s="22">
         <v>42005</v>
       </c>
@@ -6067,7 +6065,7 @@
         <v>4.3273922705466896</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="13.5">
+    <row r="63" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A63" s="22">
         <v>42036</v>
       </c>
@@ -6075,7 +6073,7 @@
         <v>4.6031119478975802</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="13.5">
+    <row r="64" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A64" s="22">
         <v>42064</v>
       </c>
@@ -6083,7 +6081,7 @@
         <v>5.0829676338002798</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="13.5">
+    <row r="65" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A65" s="22">
         <v>42095</v>
       </c>
@@ -6091,7 +6089,7 @@
         <v>6.4667750234669299</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="13.5">
+    <row r="66" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A66" s="22">
         <v>42125</v>
       </c>
@@ -6099,7 +6097,7 @@
         <v>6.3986938507038698</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="13.5">
+    <row r="67" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A67" s="22">
         <v>42156</v>
       </c>
@@ -6107,7 +6105,7 @@
         <v>6.1809177607898498</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="13.5">
+    <row r="68" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A68" s="22">
         <v>42186</v>
       </c>
@@ -6115,7 +6113,7 @@
         <v>5.9568057736049598</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="13.5">
+    <row r="69" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A69" s="22">
         <v>42217</v>
       </c>
@@ -6123,7 +6121,7 @@
         <v>6.5252645229648296</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="13.5">
+    <row r="70" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A70" s="22">
         <v>42248</v>
       </c>
@@ -6131,7 +6129,7 @@
         <v>7.0890939205032497</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="13.5">
+    <row r="71" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A71" s="22">
         <v>42278</v>
       </c>
@@ -6139,7 +6137,7 @@
         <v>7.2983346950786201</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="13.5">
+    <row r="72" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A72" s="22">
         <v>42309</v>
       </c>
@@ -6147,7 +6145,7 @@
         <v>7.3831207702299197</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="13.5">
+    <row r="73" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A73" s="22">
         <v>42339</v>
       </c>
@@ -6155,7 +6153,7 @@
         <v>7.11066751860516</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="13.5">
+    <row r="74" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A74" s="22">
         <v>42370</v>
       </c>
@@ -6163,7 +6161,7 @@
         <v>7.2269544863709898</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="13.5">
+    <row r="75" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A75" s="22">
         <v>42401</v>
       </c>
@@ -6171,7 +6169,7 @@
         <v>7.5371569309312703</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="13.5">
+    <row r="76" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A76" s="22">
         <v>42430</v>
       </c>
@@ -6179,7 +6177,7 @@
         <v>8.1894687698776192</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="13.5">
+    <row r="77" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A77" s="22">
         <v>42461</v>
       </c>
@@ -6187,7 +6185,7 @@
         <v>8.1885580354346494</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="13.5">
+    <row r="78" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A78" s="22">
         <v>42491</v>
       </c>
@@ -6195,7 +6193,7 @@
         <v>8.8338166133408595</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="13.5">
+    <row r="79" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A79" s="22">
         <v>42522</v>
       </c>
@@ -6203,7 +6201,7 @@
         <v>9.1506479832026208</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="13.5">
+    <row r="80" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A80" s="22">
         <v>42552</v>
       </c>
@@ -6211,7 +6209,7 @@
         <v>9.3593856654068599</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="13.5">
+    <row r="81" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A81" s="22">
         <v>42583</v>
       </c>
@@ -6219,7 +6217,7 @@
         <v>9.65030873622573</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="13.5">
+    <row r="82" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A82" s="22">
         <v>42614</v>
       </c>
@@ -6227,7 +6225,7 @@
         <v>9.8033316552912204</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="13.5">
+    <row r="83" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A83" s="22">
         <v>42644</v>
       </c>
@@ -6235,7 +6233,7 @@
         <v>9.5041032887436501</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="13.5">
+    <row r="84" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A84" s="22">
         <v>42675</v>
       </c>
@@ -6243,7 +6241,7 @@
         <v>10.057666239766</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="13.5">
+    <row r="85" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A85" s="22">
         <v>42705</v>
       </c>
@@ -6251,7 +6249,7 @@
         <v>9.8413566355226596</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="13.5">
+    <row r="86" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A86" s="22">
         <v>42736</v>
       </c>
@@ -6259,7 +6257,7 @@
         <v>10.0291643321797</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="13.5">
+    <row r="87" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A87" s="22">
         <v>42767</v>
       </c>
@@ -6267,7 +6265,7 @@
         <v>10.0455209193561</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="13.5">
+    <row r="88" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A88" s="22">
         <v>42795</v>
       </c>
@@ -6275,7 +6273,7 @@
         <v>9.8796224563948893</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="13.5">
+    <row r="89" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A89" s="22">
         <v>42826</v>
       </c>
@@ -6283,7 +6281,7 @@
         <v>9.0089842840891698</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="13.5">
+    <row r="90" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A90" s="22">
         <v>42856</v>
       </c>
@@ -6291,7 +6289,7 @@
         <v>9.4113081348769292</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="13.5">
+    <row r="91" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A91" s="22">
         <v>42887</v>
       </c>
@@ -6299,7 +6297,7 @@
         <v>9.9782668511723092</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="13.5">
+    <row r="92" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A92" s="22">
         <v>42917</v>
       </c>
@@ -6307,7 +6305,7 @@
         <v>10.0741836397578</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="13.5">
+    <row r="93" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A93" s="22">
         <v>42948</v>
       </c>
@@ -6315,7 +6313,7 @@
         <v>9.9079600630401501</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="13.5">
+    <row r="94" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A94" s="22">
         <v>42979</v>
       </c>
@@ -6323,7 +6321,7 @@
         <v>9.3740301914542208</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="13.5">
+    <row r="95" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A95" s="22">
         <v>43009</v>
       </c>
@@ -6331,7 +6329,7 @@
         <v>8.73712247148252</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="13.5">
+    <row r="96" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A96" s="22">
         <v>43040</v>
       </c>
@@ -6339,7 +6337,7 @@
         <v>8.2200425611798504</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="13.5">
+    <row r="97" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A97" s="22">
         <v>43070</v>
       </c>
@@ -6347,7 +6345,7 @@
         <v>8.0029876601476797</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="13.5">
+    <row r="98" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A98" s="22">
         <v>43101</v>
       </c>
@@ -6355,7 +6353,7 @@
         <v>8.4981699606632706</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="13.5">
+    <row r="99" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A99" s="22">
         <v>43132</v>
       </c>
@@ -6363,7 +6361,7 @@
         <v>9.1036042333538099</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="13.5">
+    <row r="100" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A100" s="22">
         <v>43160</v>
       </c>
@@ -6371,7 +6369,7 @@
         <v>9.1712660435298705</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="13.5">
+    <row r="101" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A101" s="22">
         <v>43191</v>
       </c>
@@ -6379,7 +6377,7 @@
         <v>9.59608917505882</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="13.5">
+    <row r="102" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A102" s="22">
         <v>43221</v>
       </c>
@@ -6387,7 +6385,7 @@
         <v>9.4443236757201507</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="13.5">
+    <row r="103" spans="1:2" ht="13.5" x14ac:dyDescent="0.15">
       <c r="A103" s="22">
         <v>43252</v>
       </c>
@@ -6406,18 +6404,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+    <sheetView topLeftCell="A106" workbookViewId="0">
       <selection activeCell="F119" sqref="F119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.25" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.75" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="14" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>157</v>
       </c>
@@ -6458,7 +6456,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="22">
         <v>40179</v>
       </c>
@@ -6470,7 +6468,7 @@
         <v>7.0792929000000004E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="22">
         <v>40210</v>
       </c>
@@ -6482,7 +6480,7 @@
         <v>2.3449319999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="22">
         <v>40238</v>
       </c>
@@ -6494,7 +6492,7 @@
         <v>6.7332668999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="22">
         <v>40269</v>
       </c>
@@ -6506,7 +6504,7 @@
         <v>-8.4261101000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="22">
         <v>40299</v>
       </c>
@@ -6518,7 +6516,7 @@
         <v>1.10480389999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="22">
         <v>40330</v>
       </c>
@@ -6530,7 +6528,7 @@
         <v>5.5850329999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="22">
         <v>40360</v>
       </c>
@@ -6542,7 +6540,7 @@
         <v>4.4394422000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" s="22">
         <v>40391</v>
       </c>
@@ -6554,7 +6552,7 @@
         <v>4.6569299999999897E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" s="22">
         <v>40422</v>
       </c>
@@ -6566,7 +6564,7 @@
         <v>5.7538099999999903E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11" s="22">
         <v>40452</v>
       </c>
@@ -6578,7 +6576,7 @@
         <v>-1.88442879999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" s="22">
         <v>40483</v>
       </c>
@@ -6590,7 +6588,7 @@
         <v>-4.44078719E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" s="22">
         <v>40513</v>
       </c>
@@ -6602,7 +6600,7 @@
         <v>7.8982520000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" s="22">
         <v>40544</v>
       </c>
@@ -6614,7 +6612,7 @@
         <v>2.6812823999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15" s="22">
         <v>40575</v>
       </c>
@@ -6626,7 +6624,7 @@
         <v>4.2496029999999997E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16" s="22">
         <v>40603</v>
       </c>
@@ -6638,7 +6636,7 @@
         <v>4.4003699999999998E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17" s="22">
         <v>40634</v>
       </c>
@@ -6650,7 +6648,7 @@
         <v>1.0434427E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18" s="22">
         <v>40664</v>
       </c>
@@ -6662,7 +6660,7 @@
         <v>3.0878966000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19" s="22">
         <v>40695</v>
       </c>
@@ -6674,7 +6672,7 @@
         <v>1.41690609999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20" s="22">
         <v>40725</v>
       </c>
@@ -6686,7 +6684,7 @@
         <v>-3.0745960000000002E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21" s="22">
         <v>40756</v>
       </c>
@@ -6698,7 +6696,7 @@
         <v>-1.3242533000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22" s="22">
         <v>40787</v>
       </c>
@@ -6710,7 +6708,7 @@
         <v>4.9135680000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23" s="22">
         <v>40817</v>
       </c>
@@ -6722,7 +6720,7 @@
         <v>-5.1505609999999997E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A24" s="22">
         <v>40848</v>
       </c>
@@ -6734,7 +6732,7 @@
         <v>-7.2079840000000006E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A25" s="22">
         <v>40878</v>
       </c>
@@ -6746,7 +6744,7 @@
         <v>7.7610819999999797E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A26" s="22">
         <v>40909</v>
       </c>
@@ -6758,7 +6756,7 @@
         <v>8.8598410000000002E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A27" s="22">
         <v>40940</v>
       </c>
@@ -6770,7 +6768,7 @@
         <v>9.1096800000000002E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A28" s="22">
         <v>40969</v>
       </c>
@@ -6782,7 +6780,7 @@
         <v>7.7905539999999999E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A29" s="22">
         <v>41000</v>
       </c>
@@ -6794,7 +6792,7 @@
         <v>5.4669129999999899E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A30" s="22">
         <v>41030</v>
       </c>
@@ -6806,7 +6804,7 @@
         <v>3.6782208999999899E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A31" s="22">
         <v>41061</v>
       </c>
@@ -6818,7 +6816,7 @@
         <v>2.90247199999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A32" s="22">
         <v>41091</v>
       </c>
@@ -6830,7 +6828,7 @@
         <v>0.12693201000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A33" s="22">
         <v>41122</v>
       </c>
@@ -6842,7 +6840,7 @@
         <v>-2.0089684999999999E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A34" s="22">
         <v>41153</v>
       </c>
@@ -6854,7 +6852,7 @@
         <v>5.0620634599999999E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A35" s="22">
         <v>41183</v>
       </c>
@@ -6866,7 +6864,7 @@
         <v>-5.8205663999999997E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A36" s="22">
         <v>41214</v>
       </c>
@@ -6878,7 +6876,7 @@
         <v>4.3491670000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A37" s="22">
         <v>41244</v>
       </c>
@@ -6890,7 +6888,7 @@
         <v>-1.5539730999999999E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A38" s="22">
         <v>41275</v>
       </c>
@@ -6902,7 +6900,7 @@
         <v>5.7074588999999898E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A39" s="22">
         <v>41306</v>
       </c>
@@ -6914,7 +6912,7 @@
         <v>-4.6673799999999996E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A40" s="22">
         <v>41334</v>
       </c>
@@ -6926,7 +6924,7 @@
         <v>-2.580236E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A41" s="22">
         <v>41365</v>
       </c>
@@ -6938,7 +6936,7 @@
         <v>0.115907389999999</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A42" s="22">
         <v>41395</v>
       </c>
@@ -6950,7 +6948,7 @@
         <v>4.1707067E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A43" s="22">
         <v>41426</v>
       </c>
@@ -6962,7 +6960,7 @@
         <v>7.7268249999999997E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A44" s="22">
         <v>41456</v>
       </c>
@@ -6974,7 +6972,7 @@
         <v>4.2229035999999998E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A45" s="22">
         <v>41487</v>
       </c>
@@ -6986,7 +6984,7 @@
         <v>4.5391095999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A46" s="22">
         <v>41518</v>
       </c>
@@ -6998,7 +6996,7 @@
         <v>-1.9165663999999999E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A47" s="22">
         <v>41548</v>
       </c>
@@ -7010,7 +7008,7 @@
         <v>2.5417170999999999E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A48" s="22">
         <v>41579</v>
       </c>
@@ -7022,7 +7020,7 @@
         <v>3.2886163999999898E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A49" s="22">
         <v>41609</v>
       </c>
@@ -7034,7 +7032,7 @@
         <v>5.7140043999999897E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A50" s="22">
         <v>41640</v>
       </c>
@@ -7046,7 +7044,7 @@
         <v>8.6967249999999996E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A51" s="22">
         <v>41671</v>
       </c>
@@ -7058,7 +7056,7 @@
         <v>2.6531809999999999E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A52" s="22">
         <v>41699</v>
       </c>
@@ -7070,7 +7068,7 @@
         <v>-2.9768780000000002E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A53" s="22">
         <v>41730</v>
       </c>
@@ -7082,7 +7080,7 @@
         <v>2.0955277000000001E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A54" s="22">
         <v>41760</v>
       </c>
@@ -7094,7 +7092,7 @@
         <v>5.382667E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A55" s="22">
         <v>41791</v>
       </c>
@@ -7106,7 +7104,7 @@
         <v>5.7733591999999997E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A56" s="22">
         <v>41821</v>
       </c>
@@ -7118,7 +7116,7 @@
         <v>5.9669632E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A57" s="22">
         <v>41852</v>
       </c>
@@ -7130,7 +7128,7 @@
         <v>0.115895149</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A58" s="22">
         <v>41883</v>
       </c>
@@ -7142,7 +7140,7 @@
         <v>0.108218603499999</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A59" s="22">
         <v>41913</v>
       </c>
@@ -7154,7 +7152,7 @@
         <v>-3.304704E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A60" s="22">
         <v>41944</v>
       </c>
@@ -7166,7 +7164,7 @@
         <v>-0.19648112400000001</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A61" s="22">
         <v>41974</v>
       </c>
@@ -7178,7 +7176,7 @@
         <v>0.10616161</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A62" s="22">
         <v>42005</v>
       </c>
@@ -7190,7 +7188,7 @@
         <v>6.9302170999999996E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A63" s="22">
         <v>42036</v>
       </c>
@@ -7202,7 +7200,7 @@
         <v>6.3714971999999995E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A64" s="22">
         <v>42064</v>
       </c>
@@ -7214,7 +7212,7 @@
         <v>0.10424593</v>
       </c>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A65" s="22">
         <v>42095</v>
       </c>
@@ -7226,7 +7224,7 @@
         <v>0.27224398999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A66" s="22">
         <v>42125</v>
       </c>
@@ -7238,7 +7236,7 @@
         <v>-1.05278399999999E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A67" s="22">
         <v>42156</v>
       </c>
@@ -7250,7 +7248,7 @@
         <v>-3.4034460000000002E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A68" s="22">
         <v>42186</v>
       </c>
@@ -7262,7 +7260,7 @@
         <v>-3.6258691000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A69" s="22">
         <v>42217</v>
       </c>
@@ -7274,7 +7272,7 @@
         <v>9.5430129999999905E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A70" s="22">
         <v>42248</v>
       </c>
@@ -7286,7 +7284,7 @@
         <v>8.64071327E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A71" s="22">
         <v>42278</v>
       </c>
@@ -7298,7 +7296,7 @@
         <v>2.9515869999999899E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A72" s="22">
         <v>42309</v>
       </c>
@@ -7310,7 +7308,7 @@
         <v>1.1617181000000001E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A73" s="22">
         <v>42339</v>
       </c>
@@ -7322,7 +7320,7 @@
         <v>-3.690218E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A74" s="22">
         <v>42370</v>
       </c>
@@ -7334,7 +7332,7 @@
         <v>1.63538749999999E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A75" s="22">
         <v>42401</v>
       </c>
@@ -7346,7 +7344,7 @@
         <v>4.2922982999999998E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A76" s="22">
         <v>42430</v>
       </c>
@@ -7358,7 +7356,7 @@
         <v>8.6546139999999994E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A77" s="22">
         <v>42461</v>
       </c>
@@ -7370,7 +7368,7 @@
         <v>-1.1120799999999899E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A78" s="22">
         <v>42491</v>
       </c>
@@ -7382,7 +7380,7 @@
         <v>7.8800024999999996E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A79" s="22">
         <v>42522</v>
       </c>
@@ -7394,7 +7392,7 @@
         <v>3.5865739999999903E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A80" s="22">
         <v>42552</v>
       </c>
@@ -7406,7 +7404,7 @@
         <v>2.2811246E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A81" s="22">
         <v>42583</v>
       </c>
@@ -7418,7 +7416,7 @@
         <v>3.1083564800000001E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A82" s="22">
         <v>42614</v>
       </c>
@@ -7430,7 +7428,7 @@
         <v>1.5856789999999999E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A83" s="22">
         <v>42644</v>
       </c>
@@ -7442,7 +7440,7 @@
         <v>-3.0523129999999999E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:14">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A84" s="22">
         <v>42675</v>
       </c>
@@ -7454,7 +7452,7 @@
         <v>5.8244627E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A85" s="22">
         <v>42705</v>
       </c>
@@ -7466,7 +7464,7 @@
         <v>-2.1506938E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A86" s="22">
         <v>42736</v>
       </c>
@@ -7478,7 +7476,7 @@
         <v>1.9083517000000001E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A87" s="22">
         <v>42767</v>
       </c>
@@ -7490,7 +7488,7 @@
         <v>1.6309022999999999E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A88" s="22">
         <v>42795</v>
       </c>
@@ -7502,7 +7500,7 @@
         <v>-1.6514669999999902E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:14">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A89" s="22">
         <v>42826</v>
       </c>
@@ -7514,7 +7512,7 @@
         <v>-8.8124639999999893E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:14">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A90" s="22">
         <v>42856</v>
       </c>
@@ -7526,7 +7524,7 @@
         <v>4.4658070000000001E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:14">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A91" s="22">
         <v>42887</v>
       </c>
@@ -7538,7 +7536,7 @@
         <v>6.0242285999999999E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A92" s="22">
         <v>42917</v>
       </c>
@@ -7550,7 +7548,7 @@
         <v>9.6125699999999904E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A93" s="22">
         <v>42948</v>
       </c>
@@ -7562,7 +7560,7 @@
         <v>-1.6499955E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A94" s="22">
         <v>42979</v>
       </c>
@@ -7574,7 +7572,7 @@
         <v>-5.3888980999999898E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A95" s="22">
         <v>43009</v>
       </c>
@@ -7586,7 +7584,7 @@
         <v>-6.7943851999999999E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A96" s="22">
         <v>43040</v>
       </c>
@@ -7598,7 +7596,7 @@
         <v>-5.9181945999999999E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:14">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A97" s="22">
         <v>43070</v>
       </c>
@@ -7610,7 +7608,7 @@
         <v>-2.6405569E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:14">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A98" s="22">
         <v>43101</v>
       </c>
@@ -7622,7 +7620,7 @@
         <v>6.1874680000000001E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:14">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A99" s="22">
         <v>43132</v>
       </c>
@@ -7634,7 +7632,7 @@
         <v>7.1242899999999998E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:14">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A100" s="22">
         <v>43160</v>
       </c>
@@ -7646,7 +7644,7 @@
         <v>7.4324199999999899E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:14">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A101" s="22">
         <v>43191</v>
       </c>
@@ -7658,7 +7656,7 @@
         <v>4.6321099999999997E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:14">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A102" s="22">
         <v>43221</v>
       </c>
@@ -7670,7 +7668,7 @@
         <v>-1.5815348999999999E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:14">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A103" s="22">
         <v>43252</v>
       </c>
@@ -7682,7 +7680,7 @@
         <v>-8.5131999999999899E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:14">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.15">
       <c r="C105" s="1" t="str">
         <f>C1</f>
         <v>1月</v>
@@ -7732,7 +7730,7 @@
         <v>12月</v>
       </c>
     </row>
-    <row r="106" spans="1:14">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B106" s="1" t="s">
         <v>173</v>
       </c>

</xml_diff>